<commit_message>
Correct description sinuositeit in krw-v_omschrijving_stuurvariabelen.xlsx
</commit_message>
<xml_diff>
--- a/data/krw-v_omschrijving_stuurvariabelen.xlsx
+++ b/data/krw-v_omschrijving_stuurvariabelen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/pydir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/krwv-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD1A159-1427-447E-BD61-BC4B05B7086B}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C924D2D-9C4F-41C8-A0F9-8C3C185E395D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Zomergemiddelde (juli-september) stroomsnelheid (cm/s); of Zomergemiddelde stroomsnelheid 0,05Q (cm/s)</t>
   </si>
   <si>
-    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Gestrekt (1.05&lt;sinuositeit≤1,25); 4 = Gestrekt (1.25&lt;sinuositeit≤1,5); 5 = Gestrekt (sinuositeit&gt;1,5)</t>
-  </si>
-  <si>
     <t>- (Percentage nat profiel gamaaid / 200)</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Maximale fractie msPAF (multi-substance Potentially Affected Fraction) per jaar op basis van gecombineerde toxische druk op ecosysteem volgens ESF Toxiciteit (-)</t>
+  </si>
+  <si>
+    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Zwak slingerend (1.05&lt;sinuositeit≤1,25); 4 = Slingerend (1.25&lt;sinuositeit≤1,5); 5 = Meanderend (sinuositeit&gt;1,5)</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +661,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -683,7 +683,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -711,13 +711,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -739,13 +739,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -767,13 +767,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,13 +781,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,13 +809,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,13 +823,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,13 +837,13 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -865,13 +865,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,13 +879,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,13 +893,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -921,7 +921,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -935,7 +935,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -949,7 +949,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -963,7 +963,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -977,13 +977,13 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1005,7 +1005,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -1019,7 +1019,7 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -1033,7 +1033,7 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1047,7 +1047,7 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -1061,13 +1061,13 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,13 +1075,13 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typos in stuurvariabelen
</commit_message>
<xml_diff>
--- a/data/krw-v_omschrijving_stuurvariabelen.xlsx
+++ b/data/krw-v_omschrijving_stuurvariabelen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/krwv-app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/pydir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C924D2D-9C4F-41C8-A0F9-8C3C185E395D}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A582B15-7D6E-4B3C-9E99-0C3B90B9944F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
     <t>Zomergemiddelde (juli-september) stroomsnelheid (cm/s); of Zomergemiddelde stroomsnelheid 0,05Q (cm/s)</t>
   </si>
   <si>
-    <t>- (Percentage nat profiel gamaaid / 200)</t>
+    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Gestrekt (1.05&lt;sinuositeit≤1,25); 4 = Gestrekt (1.25&lt;sinuositeit≤1,5); 5 = Gestrekt (sinuositeit&gt;1,5)</t>
   </si>
   <si>
     <t>Omschrijving</t>
@@ -254,7 +254,7 @@
     <t>Maximale fractie msPAF (multi-substance Potentially Affected Fraction) per jaar op basis van gecombineerde toxische druk op ecosysteem volgens ESF Toxiciteit (-)</t>
   </si>
   <si>
-    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Zwak slingerend (1.05&lt;sinuositeit≤1,25); 4 = Slingerend (1.25&lt;sinuositeit≤1,5); 5 = Meanderend (sinuositeit&gt;1,5)</t>
+    <t>(- Percentage nat profiel gemaaid / 200)</t>
   </si>
 </sst>
 </file>
@@ -317,6 +317,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,19 +642,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0377DC64-4B4C-47B0-ABB2-E1C509E85E10}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="124.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="184.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="184.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -664,7 +668,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -678,7 +682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -692,7 +696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -706,7 +710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -720,7 +724,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -734,7 +738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -748,7 +752,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -762,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -773,10 +777,10 @@
         <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -790,7 +794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -804,7 +808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -818,7 +822,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -832,7 +836,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -843,10 +847,10 @@
         <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -860,7 +864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -874,7 +878,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -888,7 +892,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -902,7 +906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -916,7 +920,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -930,7 +934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -944,7 +948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -958,7 +962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -972,7 +976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -986,7 +990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Repair typos in krw-v_omschrijving_stuurvariabelen.xlsx
</commit_message>
<xml_diff>
--- a/data/krw-v_omschrijving_stuurvariabelen.xlsx
+++ b/data/krw-v_omschrijving_stuurvariabelen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/pydir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_korving_deltares_nl/Documents/projects/11208066.002 - KRW-V regionaal/krwv-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A582B15-7D6E-4B3C-9E99-0C3B90B9944F}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{887BA769-A7AF-4AED-BE51-717711338E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{968448A4-CFD6-4C69-A4FB-65998D1D7355}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C45C5668-75CE-4BF4-A60E-179047793A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Zomergemiddelde (juli-september) stroomsnelheid (cm/s); of Zomergemiddelde stroomsnelheid 0,05Q (cm/s)</t>
   </si>
   <si>
-    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Gestrekt (1.05&lt;sinuositeit≤1,25); 4 = Gestrekt (1.25&lt;sinuositeit≤1,5); 5 = Gestrekt (sinuositeit&gt;1,5)</t>
-  </si>
-  <si>
     <t>Omschrijving</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>(- Percentage nat profiel gemaaid / 200)</t>
+  </si>
+  <si>
+    <t>1 = Recht (sinuositeit=1); 2 = Gestrekt (1&lt;sinuositeit≤1,05);  3 = Zwak slingerend (1.05&lt;sinuositeit≤1,25); 4 = Slingerend (1.25&lt;sinuositeit≤1,5); 5 = Meanderend (sinuositeit&gt;1,5)</t>
   </si>
 </sst>
 </file>
@@ -317,10 +317,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -643,18 +639,18 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="124.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="184.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="184.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -665,15 +661,15 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -682,12 +678,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -696,12 +692,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -710,26 +706,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -738,26 +734,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -766,96 +762,96 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -864,54 +860,54 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -920,12 +916,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -934,12 +930,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -948,12 +944,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
@@ -962,12 +958,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -976,26 +972,26 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1004,12 +1000,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -1018,12 +1014,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -1032,12 +1028,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1046,12 +1042,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -1060,32 +1056,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>